<commit_message>
Guest and Admin Bug Report
last ticket : 65
maintenance/add client
following the system flow


Signed-off-by: Eugene Grava <eugenegrava.c@gmail.com>
</commit_message>
<xml_diff>
--- a/bug report/Capstone Bug Report.xlsx
+++ b/bug report/Capstone Bug Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="236">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -52,7 +52,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>localhost/web/rems_copyright</t>
+    <t>localhost/rems_copyright</t>
   </si>
   <si>
     <t>Fail</t>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Guest Module</t>
   </si>
   <si>
     <t>check all links if working – user/guest/index.php </t>
@@ -229,6 +232,9 @@
     <t>high</t>
   </si>
   <si>
+    <t>Admin Module</t>
+  </si>
+  <si>
     <t>Admin Login</t>
   </si>
   <si>
@@ -599,91 +605,223 @@
     <t>error</t>
   </si>
   <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>admin footer – transactions/deploy applicant</t>
+  </si>
+  <si>
+    <t>55. click deploy applicant in the footer</t>
+  </si>
+  <si>
+    <t>redirect to employedApplicant.php</t>
+  </si>
+  <si>
+    <t>redirected to a broker link (deploy.php)</t>
+  </si>
+  <si>
+    <t>error </t>
+  </si>
+  <si>
+    <t>admin footer – transactions/performance evaluation</t>
+  </si>
+  <si>
+    <t>56. click performance evaluation from the footer</t>
+  </si>
+  <si>
+    <t>admin footer – reports/client</t>
+  </si>
+  <si>
+    <t>57. click client in the footer</t>
+  </si>
+  <si>
+    <t>admin footer – reports/applicant</t>
+  </si>
+  <si>
+    <t>58. click the applicant in the footer</t>
+  </si>
+  <si>
+    <t>redirect to applicant report</t>
+  </si>
+  <si>
+    <t>admin footer – reports/endorsement</t>
+  </si>
+  <si>
+    <t>59. click endorsement in the footer</t>
+  </si>
+  <si>
+    <t>redirect to endorsement report</t>
+  </si>
+  <si>
+    <t>admin footer – reports/employee</t>
+  </si>
+  <si>
+    <t>60. click employee in the footer</t>
+  </si>
+  <si>
+    <t>admin footer – utilities/settings</t>
+  </si>
+  <si>
+    <t>61. click settings in the footer</t>
+  </si>
+  <si>
+    <t>admin footer – utilities/website content</t>
+  </si>
+  <si>
+    <t>62. click website content</t>
+  </si>
+  <si>
+    <t>redirect to website content</t>
+  </si>
+  <si>
+    <t>broken link</t>
+  </si>
+  <si>
+    <t>admin footer – queries/queries</t>
+  </si>
+  <si>
+    <t>63. click queries in the footer</t>
+  </si>
+  <si>
+    <t>admin footer – developers/view developers</t>
+  </si>
+  <si>
+    <t>64. click view developers in the footer</t>
+  </si>
+  <si>
+    <t>redirected to a broken link (developers.php)</t>
+  </si>
+  <si>
+    <t>Admin Maintenance</t>
+  </si>
+  <si>
+    <t>add new client via admin</t>
+  </si>
+  <si>
+    <t>from user/admin
+1. click maintenace/client
+2. click add client</t>
+  </si>
+  <si>
+    <t>3. fill up form</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1. client name: sample client 001
+2. type of business: others
+3. type specific business type: pharmaceutical
+4. blk no: 001
+5. street name: Masagana
+6. subdivision: Maginhawa
+7. Barangay: Masipag
+8. District name: Sta. Mesa
+9. City: Quezon City
+10. Province: Metro Manila
+11. Country: Philippines
+12. Zip Code: 1111
+13. email: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>egrava.ojt@ayannah.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>14. select device: mobile
+15. number: 09999999999
+16. notes: &lt;blank&gt;
+17. click next</t>
+    </r>
+  </si>
+  <si>
+    <t>redirect to client contact person</t>
+  </si>
+  <si>
+    <t>4. click next</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1. last name: delos reyes
+2. first name: justine
+3. middle name: &lt;blank&gt;
+4. name ext: &lt;blank&gt;
+5. position of contact person: manager
+6. email address: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>sing.bookmark@yahoo.com
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>7. click submit</t>
+    </r>
+  </si>
+  <si>
+    <t>redirect to clientAddDone.php</t>
+  </si>
+  <si>
+    <t>email validation</t>
+  </si>
+  <si>
+    <t>5. click click here to continue browsing</t>
+  </si>
+  <si>
+    <t>redirect to guest index page</t>
+  </si>
+  <si>
     <t>medium</t>
   </si>
   <si>
-    <t>admin footer – transactions/deploy applicant</t>
-  </si>
-  <si>
-    <t>55. click deploy applicant in the footer</t>
-  </si>
-  <si>
-    <t>redirect to employedApplicant.php</t>
-  </si>
-  <si>
-    <t>redirected to a broker link (deploy.php)</t>
-  </si>
-  <si>
-    <t>error </t>
-  </si>
-  <si>
-    <t>admin footer – transactions/performance evaluation</t>
-  </si>
-  <si>
-    <t>56. click performance evaluation from the footer</t>
-  </si>
-  <si>
-    <t>admin footer – reports/client</t>
-  </si>
-  <si>
-    <t>57. click client in the footer</t>
-  </si>
-  <si>
-    <t>admin footer – reports/applicant</t>
-  </si>
-  <si>
-    <t>58. click the applicant in the footer</t>
-  </si>
-  <si>
-    <t>redirect to applicant report</t>
-  </si>
-  <si>
-    <t>admin footer – reports/endorsement</t>
-  </si>
-  <si>
-    <t>59. click endorsement in the footer</t>
-  </si>
-  <si>
-    <t>redirect to endorsement report</t>
-  </si>
-  <si>
-    <t>admin footer – reports/employee</t>
-  </si>
-  <si>
-    <t>60. click employee in the footer</t>
-  </si>
-  <si>
-    <t>admin footer – utilities/settings</t>
-  </si>
-  <si>
-    <t>61. click settings in the footer</t>
-  </si>
-  <si>
-    <t>admin footer – utilities/website content</t>
-  </si>
-  <si>
-    <t>62. click website content</t>
-  </si>
-  <si>
-    <t>redirect to website content</t>
-  </si>
-  <si>
-    <t>broken link</t>
-  </si>
-  <si>
-    <t>admin footer – queries/queries</t>
-  </si>
-  <si>
-    <t>63. click queries in the footer</t>
-  </si>
-  <si>
-    <t>admin footer – developers/view developers</t>
-  </si>
-  <si>
-    <t>64. click view developers in the footer</t>
-  </si>
-  <si>
-    <t>redirected to a broken link (developers.php)</t>
+    <t>redirection</t>
+  </si>
+  <si>
+    <t>result of add clien via admin</t>
+  </si>
+  <si>
+    <t>1. click  maintenace/client</t>
+  </si>
+  <si>
+    <t>new client named sample client 001 should appear</t>
+  </si>
+  <si>
+    <t>no new client was added</t>
   </si>
 </sst>
 </file>
@@ -694,7 +832,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -748,13 +886,28 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,7 +917,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD99594"/>
-        <bgColor rgb="FFFF99CC"/>
+        <bgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
     <fill>
@@ -783,6 +936,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6666"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -827,7 +986,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -876,6 +1035,18 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -884,8 +1055,52 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -897,6 +1112,16 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -920,7 +1145,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFD99594"/>
+      <rgbColor rgb="FFFF6666"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -936,7 +1161,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF92CDDC"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFD99594"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -965,10 +1190,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L65"/>
+  <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K65" activeCellId="0" sqref="K65"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1013,29 +1238,29 @@
         <v>5</v>
       </c>
       <c r="E2" s="6" t="n">
-        <f aca="false">COUNTIF(H7:H207,"Pass")</f>
-        <v>53</v>
+        <f aca="false">COUNTIF(H9:H214,"Pass")</f>
+        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="6" t="n">
-        <f aca="false">COUNTIF(I7:I24,"Defect")</f>
+        <f aca="false">COUNTIF(I9:I29,"Defect")</f>
         <v>0</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="6" t="n">
-        <f aca="false">COUNTIF(J7:J24,"Major")</f>
+        <f aca="false">COUNTIF(J9:J29,"Major")</f>
         <v>0</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K2" s="6" t="n">
-        <f aca="false">COUNTIF(K6:K166,"Fixed")</f>
-        <v>54</v>
+        <f aca="false">COUNTIF(K8:K173,"Fixed")</f>
+        <v>57</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,28 +1275,28 @@
         <v>11</v>
       </c>
       <c r="E3" s="6" t="n">
-        <f aca="false">COUNTIF(H6:H252,"Fail")</f>
-        <v>6</v>
+        <f aca="false">COUNTIF(H8:H259,"Fail")</f>
+        <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="6" t="n">
-        <f aca="false">COUNTIF(I6:I158,"Enhancement")</f>
+        <f aca="false">COUNTIF(I8:I165,"Enhancement")</f>
         <v>0</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="6" t="n">
-        <f aca="false">COUNTIF(J7:J24,"Minor")</f>
+        <f aca="false">COUNTIF(J9:J29,"Minor")</f>
         <v>0</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="6" t="n">
-        <f aca="false">COUNTIF(K7:K24,"Reopen")</f>
+        <f aca="false">COUNTIF(K9:K29,"Reopen")</f>
         <v>0</v>
       </c>
     </row>
@@ -1083,21 +1308,21 @@
         <v>15</v>
       </c>
       <c r="E4" s="6" t="n">
-        <f aca="false">COUNTIF(H6:H207,"Pending")</f>
+        <f aca="false">COUNTIF(H8:H214,"Pending")</f>
         <v>0</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="6" t="n">
-        <f aca="false">COUNTIF(I6:I138,"Task")</f>
+        <f aca="false">COUNTIF(I8:I145,"Task")</f>
         <v>0</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="6" t="n">
-        <f aca="false">COUNTIF(J7:J24,"Critical")</f>
+        <f aca="false">COUNTIF(J9:J29,"Critical")</f>
         <v>0</v>
       </c>
       <c r="J4" s="9"/>
@@ -1141,1988 +1366,2242 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+    </row>
+    <row r="7" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="C8" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="13" t="n">
+      <c r="E8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="16" t="n">
         <v>42426</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="13" t="n">
-        <v>42426</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="13" t="n">
-        <v>42426</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="13" t="n">
+        <v>39</v>
+      </c>
+      <c r="G9" s="16" t="n">
         <v>42426</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="13" t="n">
+        <v>41</v>
+      </c>
+      <c r="G10" s="16" t="n">
         <v>42426</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="13" t="n">
+        <v>43</v>
+      </c>
+      <c r="G11" s="16" t="n">
         <v>42426</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="13" t="n">
+        <v>45</v>
+      </c>
+      <c r="G12" s="16" t="n">
         <v>42426</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="16" t="n">
+        <v>42426</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="13" t="n">
+      <c r="E14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="16" t="n">
         <v>42426</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="13" t="n">
-        <v>42426</v>
-      </c>
       <c r="H14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="16" t="n">
+        <v>42426</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G15" s="13" t="n">
+      <c r="E16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="16" t="n">
         <v>42426</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="13" t="n">
-        <v>42426</v>
-      </c>
       <c r="H16" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="G17" s="13" t="n">
+        <v>51</v>
+      </c>
+      <c r="G17" s="16" t="n">
         <v>42426</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="16" t="n">
+        <v>42426</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="16" t="n">
+        <v>42426</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="13" t="n">
+      <c r="E20" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="16" t="n">
         <v>42426</v>
       </c>
-      <c r="H18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="H20" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="13" t="n">
+      <c r="E21" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="16" t="n">
         <v>42426</v>
       </c>
-      <c r="H19" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="H21" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" s="20" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="12" t="s">
+      <c r="B22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="C22" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H20" s="0" t="s">
+      <c r="D22" s="19"/>
+      <c r="E22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="F22" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H22" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="I22" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="J22" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="L22" s="19"/>
+    </row>
+    <row r="23" s="14" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="G23" s="24"/>
+    </row>
+    <row r="24" s="14" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="G25" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L25" s="0" t="s">
-        <v>84</v>
-      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="G24" s="24"/>
+    </row>
+    <row r="25" s="14" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="G25" s="24"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="13" t="n">
+        <v>70</v>
+      </c>
+      <c r="G26" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L26" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>90</v>
+        <v>72</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="13" t="n">
+        <v>74</v>
+      </c>
+      <c r="G27" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="0" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="G28" s="13" t="n">
+        <v>76</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" s="13" t="n">
+        <v>81</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L29" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>101</v>
+        <v>20</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="G30" s="13" t="n">
+        <v>85</v>
+      </c>
+      <c r="G30" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="13" t="n">
+        <v>89</v>
+      </c>
+      <c r="G31" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="G32" s="13" t="n">
+        <v>93</v>
+      </c>
+      <c r="G32" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J32" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="G33" s="13" t="n">
+        <v>97</v>
+      </c>
+      <c r="G33" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>114</v>
+        <v>37</v>
+      </c>
+      <c r="L33" s="26" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="G34" s="13" t="n">
+        <v>101</v>
+      </c>
+      <c r="G34" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J34" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="G35" s="13" t="n">
+        <v>104</v>
+      </c>
+      <c r="G35" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="G36" s="13" t="n">
+        <v>108</v>
+      </c>
+      <c r="G36" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" s="13" t="n">
+        <v>112</v>
+      </c>
+      <c r="G37" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="13" t="n">
+        <v>115</v>
+      </c>
+      <c r="G38" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J38" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K38" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L38" s="0" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="13" t="n">
+        <v>119</v>
+      </c>
+      <c r="G39" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J39" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K39" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L39" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="13" t="n">
+        <v>123</v>
+      </c>
+      <c r="G40" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J40" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K40" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L40" s="0" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="G41" s="13" t="n">
+        <v>127</v>
+      </c>
+      <c r="G41" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K41" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="G42" s="13" t="n">
+        <v>130</v>
+      </c>
+      <c r="G42" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K42" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L42" s="0" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="G43" s="13" t="n">
+        <v>133</v>
+      </c>
+      <c r="G43" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>150</v>
+        <v>35</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>65</v>
+        <v>36</v>
+      </c>
+      <c r="K43" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="L43" s="0" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G44" s="13" t="n">
+        <v>137</v>
+      </c>
+      <c r="G44" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G45" s="13" t="n">
+        <v>140</v>
+      </c>
+      <c r="G45" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J45" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K45" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="G46" s="13" t="n">
+        <v>143</v>
+      </c>
+      <c r="G46" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K46" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L46" s="0" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="G47" s="13" t="n">
+        <v>146</v>
+      </c>
+      <c r="G47" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J47" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K47" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L47" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H48" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I48" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J48" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K48" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L48" s="0" t="s">
-        <v>118</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="n">
+        <v>38</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H48" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I48" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L48" s="20" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G49" s="13" t="n">
+        <v>155</v>
+      </c>
+      <c r="G49" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K49" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L49" s="0" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>169</v>
+        <v>89</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="G50" s="13" t="n">
+        <v>89</v>
+      </c>
+      <c r="G50" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K50" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L50" s="0" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="G51" s="13" t="n">
+        <v>160</v>
+      </c>
+      <c r="G51" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J51" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K51" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="G52" s="13" t="n">
+        <v>163</v>
+      </c>
+      <c r="G52" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J52" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K52" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>179</v>
+        <v>93</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="G53" s="13" t="n">
+        <v>93</v>
+      </c>
+      <c r="G53" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J53" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K53" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L53" s="0" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G54" s="13" t="n">
+        <v>168</v>
+      </c>
+      <c r="G54" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J54" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K54" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L54" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="G55" s="13" t="n">
+        <v>171</v>
+      </c>
+      <c r="G55" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="J55" s="0" t="s">
-        <v>187</v>
+        <v>36</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="G56" s="13" t="n">
+        <v>174</v>
+      </c>
+      <c r="G56" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>192</v>
+        <v>35</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>187</v>
+        <v>36</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="G57" s="13" t="n">
+        <v>177</v>
+      </c>
+      <c r="G57" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K57" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L57" s="0" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="G58" s="13" t="n">
+        <v>181</v>
+      </c>
+      <c r="G58" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K58" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>199</v>
+        <v>108</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="G59" s="13" t="n">
+        <v>108</v>
+      </c>
+      <c r="G59" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J59" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>200</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="E60" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="F60" s="0" t="s">
-        <v>202</v>
-      </c>
-      <c r="G60" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H60" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I60" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J60" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K60" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L60" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>204</v>
-      </c>
-      <c r="E61" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="F61" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="G61" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H61" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="I61" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J61" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="L61" s="0" t="s">
-        <v>176</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="17" t="n">
+        <v>50</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="G60" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I60" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="17" t="n">
+        <v>51</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="G61" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H61" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I61" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G62" s="13" t="n">
+        <v>119</v>
+      </c>
+      <c r="G62" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J62" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L62" s="0" t="s">
-        <v>176</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>209</v>
+        <v>133</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="G63" s="13" t="n">
+        <v>133</v>
+      </c>
+      <c r="G63" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>186</v>
+        <v>35</v>
       </c>
       <c r="J63" s="0" t="s">
-        <v>187</v>
+        <v>36</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>141</v>
+        <v>201</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="G64" s="13" t="n">
+        <v>201</v>
+      </c>
+      <c r="G64" s="16" t="n">
         <v>42427</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G65" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G66" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="G67" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="68" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="17" t="n">
+        <v>58</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G68" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I68" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="F69" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G69" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H69" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K69" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="17" t="n">
         <v>60</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>213</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="E65" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F65" s="0" t="s">
+      <c r="B70" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="G65" s="13" t="n">
-        <v>42427</v>
-      </c>
-      <c r="H65" s="0" t="s">
+      <c r="C70" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="G70" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I70" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J70" s="20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="22"/>
+      <c r="G71" s="24"/>
+    </row>
+    <row r="72" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="G72" s="24"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="25"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="G74" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="G75" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K75" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L75" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="I65" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="J65" s="0" t="s">
-        <v>187</v>
+      <c r="C76" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="G76" s="16" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K76" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L76" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="17" t="n">
+        <v>64</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G77" s="21" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H77" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I77" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="J77" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="L77" s="19" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="27" t="n">
+        <v>65</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="F78" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="G78" s="28" t="n">
+        <v>42427</v>
+      </c>
+      <c r="H78" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="I78" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J78" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="L78" s="20" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A6:C7"/>
+    <mergeCell ref="A24:C25"/>
+    <mergeCell ref="A72:C73"/>
   </mergeCells>
+  <conditionalFormatting sqref="K77:AMJ77,A77:I77">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>fail</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J77">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>fail</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G78">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>fail</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D75" r:id="rId1" display="egrava.ojt@ayannah.com"/>
+    <hyperlink ref="D76" r:id="rId2" display="sing.bookmark@yahoo.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Modified the bug report
finished all admin maintenance


Signed-off-by: Eugene Grava <eugenegrava.c@gmail.com>
</commit_message>
<xml_diff>
--- a/bug report/Capstone Bug Report.xlsx
+++ b/bug report/Capstone Bug Report.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="306">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -778,15 +778,7 @@
 2. click update client</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1. search client to update: sample client 001
+    <t>1. search client to update: sample client 001
 2. client name: edit sample client 001
 3. type of business: supermarket
 4. blk: 002
@@ -798,29 +790,10 @@
 10. Province: Metro Manila
 11. Country: Philippines
 12. Zip Code: 1111
-13. Email: eugene </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>grava.c@gmail</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> .com 
+13. Email: eugene grava.c@gmail .com 
 14. select device: mobile
 15. contact number: 0999999999
 16. click next</t>
-    </r>
   </si>
   <si>
     <t>redirect to contact person</t>
@@ -832,40 +805,13 @@
     <t>3. click next</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1. last name: delos reyes
+    <t>1. last name: delos reyes
 2. first name: justine
 3. middle name: &lt;blank&gt;
 4. name ext: &lt;blank&gt;
 5. position of contact person: Manager
-6. email address:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>sign.bookmark@yahoo.com
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>7. click update</t>
-    </r>
+6. email address:  sign.bookmark@yahoo.com
+7. click update</t>
   </si>
   <si>
     <t>update done</t>
@@ -1063,6 +1009,29 @@
   </si>
   <si>
     <t>redirected to a broken link (type of business add done.php)</t>
+  </si>
+  <si>
+    <t>update type of business</t>
+  </si>
+  <si>
+    <t>1. click update typ of business</t>
+  </si>
+  <si>
+    <t>redirected to update type of business</t>
+  </si>
+  <si>
+    <t>1. fill up update form</t>
+  </si>
+  <si>
+    <t>1. select type of business: pharmaceutical
+2. description: the number one drug store int the philippines
+3. click submit</t>
+  </si>
+  <si>
+    <t>redirected to a broken link (typeOfBusinessUpdateDone.php)</t>
+  </si>
+  <si>
+    <t>Redirection (update was done successfully)</t>
   </si>
 </sst>
 </file>
@@ -1447,21 +1416,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L95"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E100" activeCellId="0" sqref="E100"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1496,7 +1465,7 @@
       </c>
       <c r="E2" s="6" t="n">
         <f aca="false">COUNTIF(H9:H214,"Pass")</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>6</v>
@@ -1517,7 +1486,7 @@
       </c>
       <c r="K2" s="6" t="n">
         <f aca="false">COUNTIF(K8:K173,"Fixed")</f>
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,7 +1502,7 @@
       </c>
       <c r="E3" s="6" t="n">
         <f aca="false">COUNTIF(H8:H259,"Fail")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>12</v>
@@ -3839,7 +3808,7 @@
       <c r="C79" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="D79" s="14" t="s">
+      <c r="D79" s="24" t="s">
         <v>238</v>
       </c>
       <c r="E79" s="0" t="s">
@@ -3874,7 +3843,7 @@
       <c r="C80" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="D80" s="14" t="s">
+      <c r="D80" s="24" t="s">
         <v>242</v>
       </c>
       <c r="E80" s="0" t="s">
@@ -4417,6 +4386,73 @@
       </c>
       <c r="L95" s="19" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E96" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F96" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="G96" s="15" t="n">
+        <v>42428</v>
+      </c>
+      <c r="H96" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I96" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J96" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K96" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L96" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="97" s="18" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="16" t="n">
+        <v>84</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="G97" s="20" t="n">
+        <v>42428</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I97" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="J97" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="L97" s="18" t="s">
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -4528,8 +4564,8 @@
   <hyperlinks>
     <hyperlink ref="D75" r:id="rId1" display="1. client name: sample client 001&#10;2. type of business: others&#10;3. type specific business type: pharmaceutical&#10;4. blk no: 001&#10;5. street name: Masagana&#10;6. subdivision: Maginhawa&#10;7. Barangay: Masipag&#10;8. District name: Sta. Mesa&#10;9. City: Quezon City&#10;10. Province: Metro Manila&#10;11. Country: Philippines&#10;12. Zip Code: 1111&#10;13. email: egrava.ojt@ayannah.com&#10;14. select device: mobile&#10;15. number: 09999999999&#10;16. notes: &lt;blank&gt;&#10;17. click next"/>
     <hyperlink ref="D76" r:id="rId2" display="1. last name: delos reyes&#10;2. first name: justine&#10;3. middle name: &lt;blank&gt;&#10;4. name ext: &lt;blank&gt;&#10;5. position of contact person: manager&#10;6. email address: sing.bookmark@yahoo.com&#10;7. click submit"/>
-    <hyperlink ref="D79" r:id="rId3" display="grava.c@gmail"/>
-    <hyperlink ref="D80" r:id="rId4" display="sign.bookmark@yahoo.com"/>
+    <hyperlink ref="D79" r:id="rId3" display="1. search client to update: sample client 001&#10;2. client name: edit sample client 001&#10;3. type of business: supermarket&#10;4. blk: 002&#10;5. street name: masaganas&#10;6. subdivision: maginhawas&#10;7. barangay: masipags&#10;8. district name: &lt;blank&gt;&#10;9. city: Quezon City&#10;10. Province: Metro Manila&#10;11. Country: Philippines&#10;12. Zip Code: 1111&#10;13. Email: eugene grava.c@gmail .com &#10;14. select device: mobile&#10;15. contact number: 0999999999&#10;16. click next"/>
+    <hyperlink ref="D80" r:id="rId4" display="1. last name: delos reyes&#10;2. first name: justine&#10;3. middle name: &lt;blank&gt;&#10;4. name ext: &lt;blank&gt;&#10;5. position of contact person: Manager&#10;6. email address:  sign.bookmark@yahoo.com&#10;7. click update"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>